<commit_message>
saco and speedtrans sheet fixes
Former-commit-id: f926fde97d393282ca6f8386d6067bbe0498897f
</commit_message>
<xml_diff>
--- a/db/dummydata/saco/saco__hubs.xlsx
+++ b/db/dummydata/saco/saco__hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="185">
   <si>
     <t>STATUS</t>
   </si>
@@ -427,15 +427,18 @@
     <t>Cebu</t>
   </si>
   <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Mandaue City, Provinz Cebu, Philippinen</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
     <t>Philipines</t>
   </si>
   <si>
-    <t>Mandaue City, Provinz Cebu, Philippinen</t>
-  </si>
-  <si>
-    <t>Manila</t>
-  </si>
-  <si>
     <t>Port Area, Manila, Metro Manila, Philippinen</t>
   </si>
   <si>
@@ -553,7 +556,7 @@
     <t>Haiphong</t>
   </si>
   <si>
-    <t>Vietnam</t>
+    <t>Viet Nam</t>
   </si>
   <si>
     <t>Hai Phong port, Hoàng Diệu, Máy Tơ, Ngô Quyền, Haiphong, Vietnam</t>
@@ -2099,10 +2102,10 @@
         <v>120.95</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I56" s="6"/>
     </row>
@@ -2114,7 +2117,7 @@
         <v>14</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E57" s="6">
         <v>24.9895801</v>
@@ -2123,10 +2126,10 @@
         <v>51.5525819</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -2137,7 +2140,7 @@
         <v>14</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E58" s="6">
         <v>26.4876505</v>
@@ -2146,10 +2149,10 @@
         <v>50.1961209</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -2160,7 +2163,7 @@
         <v>14</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E59" s="6">
         <v>21.4499763</v>
@@ -2169,10 +2172,10 @@
         <v>39.1725733</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
@@ -2183,7 +2186,7 @@
         <v>14</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E60" s="6">
         <v>1.27371</v>
@@ -2192,10 +2195,10 @@
         <v>103.801314</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I60" s="6"/>
     </row>
@@ -2207,7 +2210,7 @@
         <v>14</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E61" s="6">
         <v>6.9270786</v>
@@ -2216,10 +2219,10 @@
         <v>79.861243</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
@@ -2230,7 +2233,7 @@
         <v>14</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E62" s="6">
         <v>35.5321529</v>
@@ -2239,10 +2242,10 @@
         <v>35.7748042</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
@@ -2253,7 +2256,7 @@
         <v>14</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E63" s="6">
         <v>22.61840502</v>
@@ -2262,10 +2265,10 @@
         <v>120.29800207</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -2276,7 +2279,7 @@
         <v>14</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E64" s="6">
         <v>25.1388806</v>
@@ -2285,10 +2288,10 @@
         <v>121.7508906</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
@@ -2299,7 +2302,7 @@
         <v>14</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E65" s="6">
         <v>24.288098</v>
@@ -2308,10 +2311,10 @@
         <v>120.5106365</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
@@ -2322,7 +2325,7 @@
         <v>14</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E66" s="6">
         <v>13.7037349</v>
@@ -2331,10 +2334,10 @@
         <v>100.5754479</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
@@ -2345,7 +2348,7 @@
         <v>14</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E67" s="6">
         <v>13.1040552</v>
@@ -2354,10 +2357,10 @@
         <v>100.9158073</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
@@ -2368,7 +2371,7 @@
         <v>14</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E68" s="6">
         <v>7.2103359</v>
@@ -2377,10 +2380,10 @@
         <v>100.5838678</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
@@ -2391,7 +2394,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E69" s="6">
         <v>24.806936</v>
@@ -2400,10 +2403,10 @@
         <v>54.644405</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
@@ -2414,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E70" s="6">
         <v>24.967303</v>
@@ -2423,10 +2426,10 @@
         <v>55.098639</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
@@ -2437,7 +2440,7 @@
         <v>14</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E71" s="6">
         <v>25.3462553</v>
@@ -2446,10 +2449,10 @@
         <v>55.4209317</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -2460,7 +2463,7 @@
         <v>14</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E72" s="6">
         <v>20.8602909</v>
@@ -2469,10 +2472,10 @@
         <v>106.7248161</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
@@ -2483,7 +2486,7 @@
         <v>14</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E73" s="6">
         <v>10.7567427</v>
@@ -2492,10 +2495,10 @@
         <v>106.7170139</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">

</xml_diff>